<commit_message>
Update data with balanced design and unbalanced design (see the excel sheet for details)
</commit_message>
<xml_diff>
--- a/USAuthors/Data/Author.design.xlsx
+++ b/USAuthors/Data/Author.design.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juchi\Box Sync\Abdi_lab\RM3\Data sets\InPrep\InClassExamples\USAuthors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9288FE9-C5F5-4865-96F0-E35924C3F74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87386417-9BC3-4B00-B735-D611E9111222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5685" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{8205C31E-2908-416D-B534-2ACEB3475067}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{8205C31E-2908-416D-B534-2ACEB3475067}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$239</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$235</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="280">
   <si>
     <t>Lincoln, Abraham</t>
   </si>
@@ -815,15 +815,6 @@
   </si>
   <si>
     <t>writer</t>
-  </si>
-  <si>
-    <t>chilren</t>
-  </si>
-  <si>
-    <t>politicain</t>
-  </si>
-  <si>
-    <t>natrualist</t>
   </si>
   <si>
     <t>16th</t>
@@ -3421,7 +3412,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B9EEEE8F-FE2C-4F2B-A432-3ACBB7449592}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B9EEEE8F-FE2C-4F2B-A432-3ACBB7449592}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:J11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -3850,8 +3841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4629592B-0E0F-485D-B1E6-ECE7C0C63CAD}">
   <dimension ref="A1:H235"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="J125" sqref="J125"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3861,7 +3852,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B1" t="s">
         <v>231</v>
@@ -3890,10 +3881,10 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" t="s">
         <v>270</v>
-      </c>
-      <c r="C2" t="s">
-        <v>273</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -3910,10 +3901,10 @@
         <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F3" t="s">
         <v>252</v>
@@ -3927,10 +3918,10 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F4" t="s">
         <v>242</v>
@@ -3944,10 +3935,10 @@
         <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F5" t="s">
         <v>245</v>
@@ -3961,10 +3952,10 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F6" t="s">
         <v>245</v>
@@ -3978,10 +3969,10 @@
         <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F7" t="s">
         <v>242</v>
@@ -3995,10 +3986,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C8" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F8" t="s">
         <v>242</v>
@@ -4012,10 +4003,10 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C9" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F9" t="s">
         <v>246</v>
@@ -4029,10 +4020,10 @@
         <v>147</v>
       </c>
       <c r="B10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F10" t="s">
         <v>253</v>
@@ -4041,7 +4032,7 @@
         <v>247</v>
       </c>
       <c r="H10" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -4049,10 +4040,10 @@
         <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F11" t="s">
         <v>240</v>
@@ -4066,10 +4057,10 @@
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C12" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F12" t="s">
         <v>246</v>
@@ -4083,10 +4074,10 @@
         <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C13" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F13" t="s">
         <v>242</v>
@@ -4100,10 +4091,10 @@
         <v>152</v>
       </c>
       <c r="B14" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C14" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F14" t="s">
         <v>248</v>
@@ -4117,10 +4108,10 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C15" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F15" t="s">
         <v>240</v>
@@ -4134,10 +4125,10 @@
         <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C16" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F16" t="s">
         <v>248</v>
@@ -4151,10 +4142,10 @@
         <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C17" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F17" t="s">
         <v>242</v>
@@ -4168,10 +4159,10 @@
         <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C18" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F18" t="s">
         <v>240</v>
@@ -4185,10 +4176,10 @@
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C19" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F19" t="s">
         <v>240</v>
@@ -4202,10 +4193,10 @@
         <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F20" t="s">
         <v>240</v>
@@ -4219,10 +4210,10 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C21" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F21" t="s">
         <v>240</v>
@@ -4236,10 +4227,10 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C22" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F22" t="s">
         <v>242</v>
@@ -4253,10 +4244,10 @@
         <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C23" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F23" t="s">
         <v>253</v>
@@ -4270,10 +4261,10 @@
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C24" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F24" t="s">
         <v>240</v>
@@ -4287,10 +4278,10 @@
         <v>108</v>
       </c>
       <c r="B25" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C25" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F25" t="s">
         <v>252</v>
@@ -4304,10 +4295,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C26" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F26" t="s">
         <v>240</v>
@@ -4321,10 +4312,10 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C27" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F27" t="s">
         <v>245</v>
@@ -4338,10 +4329,10 @@
         <v>157</v>
       </c>
       <c r="B28" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C28" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F28" t="s">
         <v>248</v>
@@ -4355,10 +4346,10 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C29" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F29" t="s">
         <v>242</v>
@@ -4372,10 +4363,10 @@
         <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C30" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F30" t="s">
         <v>253</v>
@@ -4389,10 +4380,10 @@
         <v>96</v>
       </c>
       <c r="B31" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C31" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F31" t="s">
         <v>242</v>
@@ -4406,10 +4397,10 @@
         <v>53</v>
       </c>
       <c r="B32" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C32" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F32" t="s">
         <v>242</v>
@@ -4423,10 +4414,10 @@
         <v>112</v>
       </c>
       <c r="B33" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C33" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F33" t="s">
         <v>245</v>
@@ -4440,10 +4431,10 @@
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C34" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F34" t="s">
         <v>245</v>
@@ -4457,10 +4448,10 @@
         <v>146</v>
       </c>
       <c r="B35" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C35" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F35" t="s">
         <v>242</v>
@@ -4474,10 +4465,10 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C36" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F36" t="s">
         <v>244</v>
@@ -4491,10 +4482,10 @@
         <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F37" t="s">
         <v>240</v>
@@ -4508,10 +4499,10 @@
         <v>77</v>
       </c>
       <c r="B38" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C38" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F38" t="s">
         <v>240</v>
@@ -4525,10 +4516,10 @@
         <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C39" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F39" t="s">
         <v>240</v>
@@ -4542,10 +4533,10 @@
         <v>141</v>
       </c>
       <c r="B40" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C40" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F40" t="s">
         <v>245</v>
@@ -4559,10 +4550,10 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C41" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F41" t="s">
         <v>240</v>
@@ -4576,10 +4567,10 @@
         <v>30</v>
       </c>
       <c r="B42" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C42" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F42" t="s">
         <v>246</v>
@@ -4593,10 +4584,10 @@
         <v>218</v>
       </c>
       <c r="B43" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C43" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
@@ -4613,10 +4604,10 @@
         <v>67</v>
       </c>
       <c r="B44" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C44" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F44" t="s">
         <v>240</v>
@@ -4630,10 +4621,10 @@
         <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C45" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F45" t="s">
         <v>252</v>
@@ -4647,10 +4638,10 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C46" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F46" t="s">
         <v>252</v>
@@ -4664,10 +4655,10 @@
         <v>217</v>
       </c>
       <c r="B47" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C47" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
@@ -4681,10 +4672,10 @@
         <v>36</v>
       </c>
       <c r="B48" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C48" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F48" t="s">
         <v>240</v>
@@ -4698,10 +4689,10 @@
         <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C49" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F49" t="s">
         <v>240</v>
@@ -4715,10 +4706,10 @@
         <v>172</v>
       </c>
       <c r="B50" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C50" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F50" t="s">
         <v>248</v>
@@ -4732,10 +4723,10 @@
         <v>79</v>
       </c>
       <c r="B51" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C51" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F51" t="s">
         <v>242</v>
@@ -4749,10 +4740,10 @@
         <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C52" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F52" t="s">
         <v>240</v>
@@ -4766,10 +4757,10 @@
         <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C53" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F53" t="s">
         <v>240</v>
@@ -4783,10 +4774,10 @@
         <v>102</v>
       </c>
       <c r="B54" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C54" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F54" t="s">
         <v>240</v>
@@ -4800,10 +4791,10 @@
         <v>38</v>
       </c>
       <c r="B55" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C55" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F55" t="s">
         <v>240</v>
@@ -4817,10 +4808,10 @@
         <v>160</v>
       </c>
       <c r="B56" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C56" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F56" t="s">
         <v>257</v>
@@ -4834,10 +4825,10 @@
         <v>35</v>
       </c>
       <c r="B57" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C57" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F57" t="s">
         <v>242</v>
@@ -4851,10 +4842,10 @@
         <v>37</v>
       </c>
       <c r="B58" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C58" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F58" t="s">
         <v>246</v>
@@ -4868,10 +4859,10 @@
         <v>52</v>
       </c>
       <c r="B59" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C59" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F59" t="s">
         <v>254</v>
@@ -4885,10 +4876,10 @@
         <v>139</v>
       </c>
       <c r="B60" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C60" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F60" t="s">
         <v>242</v>
@@ -4902,10 +4893,10 @@
         <v>42</v>
       </c>
       <c r="B61" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C61" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F61" t="s">
         <v>240</v>
@@ -4919,10 +4910,10 @@
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C62" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F62" t="s">
         <v>246</v>
@@ -4936,13 +4927,13 @@
         <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C63" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F63" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="G63" t="s">
         <v>241</v>
@@ -4953,10 +4944,10 @@
         <v>101</v>
       </c>
       <c r="B64" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C64" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F64" t="s">
         <v>240</v>
@@ -4970,10 +4961,10 @@
         <v>89</v>
       </c>
       <c r="B65" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C65" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F65" t="s">
         <v>240</v>
@@ -4987,10 +4978,10 @@
         <v>24</v>
       </c>
       <c r="B66" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C66" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F66" t="s">
         <v>240</v>
@@ -5004,10 +4995,10 @@
         <v>135</v>
       </c>
       <c r="B67" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C67" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F67" t="s">
         <v>242</v>
@@ -5021,10 +5012,10 @@
         <v>216</v>
       </c>
       <c r="B68" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C68" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -5035,10 +5026,10 @@
         <v>227</v>
       </c>
       <c r="B69" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C69" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -5049,10 +5040,10 @@
         <v>192</v>
       </c>
       <c r="B70" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C70" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
@@ -5063,13 +5054,13 @@
         <v>91</v>
       </c>
       <c r="B71" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C71" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F71" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="G71" t="s">
         <v>247</v>
@@ -5080,10 +5071,10 @@
         <v>27</v>
       </c>
       <c r="B72" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C72" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F72" t="s">
         <v>248</v>
@@ -5097,10 +5088,10 @@
         <v>116</v>
       </c>
       <c r="B73" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C73" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E73" t="b">
         <v>1</v>
@@ -5117,10 +5108,10 @@
         <v>26</v>
       </c>
       <c r="B74" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C74" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F74" t="s">
         <v>245</v>
@@ -5134,10 +5125,10 @@
         <v>194</v>
       </c>
       <c r="B75" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C75" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
@@ -5151,10 +5142,10 @@
         <v>119</v>
       </c>
       <c r="B76" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C76" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E76" t="b">
         <v>1</v>
@@ -5171,10 +5162,10 @@
         <v>120</v>
       </c>
       <c r="B77" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C77" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E77" t="b">
         <v>1</v>
@@ -5191,10 +5182,10 @@
         <v>85</v>
       </c>
       <c r="B78" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C78" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F78" t="s">
         <v>253</v>
@@ -5208,10 +5199,10 @@
         <v>7</v>
       </c>
       <c r="B79" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C79" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F79" t="s">
         <v>240</v>
@@ -5225,10 +5216,10 @@
         <v>118</v>
       </c>
       <c r="B80" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C80" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E80" t="b">
         <v>1</v>
@@ -5245,10 +5236,10 @@
         <v>117</v>
       </c>
       <c r="B81" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C81" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E81" t="b">
         <v>1</v>
@@ -5265,10 +5256,10 @@
         <v>43</v>
       </c>
       <c r="B82" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C82" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F82" t="s">
         <v>240</v>
@@ -5282,10 +5273,10 @@
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C83" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E83" t="b">
         <v>1</v>
@@ -5302,10 +5293,10 @@
         <v>121</v>
       </c>
       <c r="B84" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C84" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E84" t="b">
         <v>1</v>
@@ -5322,10 +5313,10 @@
         <v>3</v>
       </c>
       <c r="B85" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C85" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F85" t="s">
         <v>240</v>
@@ -5339,10 +5330,10 @@
         <v>69</v>
       </c>
       <c r="B86" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C86" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F86" t="s">
         <v>240</v>
@@ -5359,10 +5350,10 @@
         <v>15</v>
       </c>
       <c r="B87" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C87" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F87" t="s">
         <v>245</v>
@@ -5376,10 +5367,10 @@
         <v>40</v>
       </c>
       <c r="B88" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C88" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F88" t="s">
         <v>250</v>
@@ -5393,10 +5384,10 @@
         <v>45</v>
       </c>
       <c r="B89" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C89" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F89" t="s">
         <v>253</v>
@@ -5410,13 +5401,13 @@
         <v>81</v>
       </c>
       <c r="B90" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C90" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F90" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="G90" t="s">
         <v>241</v>
@@ -5427,10 +5418,10 @@
         <v>13</v>
       </c>
       <c r="B91" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C91" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F91" t="s">
         <v>240</v>
@@ -5444,10 +5435,10 @@
         <v>104</v>
       </c>
       <c r="B92" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C92" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F92" t="s">
         <v>253</v>
@@ -5461,10 +5452,10 @@
         <v>131</v>
       </c>
       <c r="B93" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C93" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E93" t="b">
         <v>1</v>
@@ -5481,10 +5472,10 @@
         <v>129</v>
       </c>
       <c r="B94" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C94" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E94" t="b">
         <v>1</v>
@@ -5501,10 +5492,10 @@
         <v>122</v>
       </c>
       <c r="B95" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C95" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E95" t="b">
         <v>1</v>
@@ -5521,10 +5512,10 @@
         <v>16</v>
       </c>
       <c r="B96" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C96" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F96" t="s">
         <v>242</v>
@@ -5538,10 +5529,10 @@
         <v>125</v>
       </c>
       <c r="B97" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C97" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E97" t="b">
         <v>1</v>
@@ -5558,10 +5549,10 @@
         <v>78</v>
       </c>
       <c r="B98" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C98" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F98" t="s">
         <v>242</v>
@@ -5575,10 +5566,10 @@
         <v>65</v>
       </c>
       <c r="B99" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C99" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F99" t="s">
         <v>240</v>
@@ -5592,10 +5583,10 @@
         <v>162</v>
       </c>
       <c r="B100" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C100" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F100" t="s">
         <v>242</v>
@@ -5609,10 +5600,10 @@
         <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C101" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F101" t="s">
         <v>242</v>
@@ -5626,10 +5617,10 @@
         <v>123</v>
       </c>
       <c r="B102" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C102" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E102" t="b">
         <v>1</v>
@@ -5646,13 +5637,13 @@
         <v>107</v>
       </c>
       <c r="B103" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C103" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F103" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G103" t="s">
         <v>241</v>
@@ -5663,10 +5654,10 @@
         <v>58</v>
       </c>
       <c r="B104" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C104" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F104" t="s">
         <v>248</v>
@@ -5680,10 +5671,10 @@
         <v>127</v>
       </c>
       <c r="B105" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C105" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E105" t="b">
         <v>1</v>
@@ -5700,10 +5691,10 @@
         <v>80</v>
       </c>
       <c r="B106" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C106" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F106" t="s">
         <v>240</v>
@@ -5717,10 +5708,10 @@
         <v>126</v>
       </c>
       <c r="B107" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C107" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E107" t="b">
         <v>1</v>
@@ -5737,10 +5728,10 @@
         <v>34</v>
       </c>
       <c r="B108" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C108" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F108" t="s">
         <v>240</v>
@@ -5754,10 +5745,10 @@
         <v>170</v>
       </c>
       <c r="B109" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C109" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F109" t="s">
         <v>240</v>
@@ -5771,10 +5762,10 @@
         <v>44</v>
       </c>
       <c r="B110" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C110" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F110" t="s">
         <v>252</v>
@@ -5788,10 +5779,10 @@
         <v>128</v>
       </c>
       <c r="B111" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C111" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E111" t="b">
         <v>1</v>
@@ -5808,10 +5799,10 @@
         <v>130</v>
       </c>
       <c r="B112" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C112" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E112" t="b">
         <v>1</v>
@@ -5828,10 +5819,10 @@
         <v>84</v>
       </c>
       <c r="B113" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C113" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F113" t="s">
         <v>240</v>
@@ -5845,10 +5836,10 @@
         <v>191</v>
       </c>
       <c r="B114" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C114" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D114" t="b">
         <v>0</v>
@@ -5865,10 +5856,10 @@
         <v>153</v>
       </c>
       <c r="B115" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C115" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F115" t="s">
         <v>248</v>
@@ -5882,10 +5873,10 @@
         <v>136</v>
       </c>
       <c r="B116" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C116" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F116" t="s">
         <v>240</v>
@@ -5899,10 +5890,10 @@
         <v>124</v>
       </c>
       <c r="B117" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C117" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E117" t="b">
         <v>1</v>
@@ -5919,10 +5910,10 @@
         <v>14</v>
       </c>
       <c r="B118" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C118" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F118" t="s">
         <v>240</v>
@@ -5936,10 +5927,10 @@
         <v>182</v>
       </c>
       <c r="B119" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C119" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D119" t="b">
         <v>0</v>
@@ -5956,10 +5947,10 @@
         <v>29</v>
       </c>
       <c r="B120" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C120" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F120" t="s">
         <v>240</v>
@@ -5973,10 +5964,10 @@
         <v>133</v>
       </c>
       <c r="B121" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C121" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E121" t="b">
         <v>1</v>
@@ -5993,10 +5984,10 @@
         <v>32</v>
       </c>
       <c r="B122" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C122" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F122" t="s">
         <v>240</v>
@@ -6010,10 +6001,10 @@
         <v>132</v>
       </c>
       <c r="B123" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C123" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E123" t="b">
         <v>1</v>
@@ -6022,7 +6013,7 @@
         <v>238</v>
       </c>
       <c r="G123" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
@@ -6030,10 +6021,10 @@
         <v>148</v>
       </c>
       <c r="B124" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C124" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E124" t="b">
         <v>1</v>
@@ -6042,7 +6033,7 @@
         <v>238</v>
       </c>
       <c r="G124" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
@@ -6050,16 +6041,16 @@
         <v>226</v>
       </c>
       <c r="B125" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C125" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D125" t="b">
         <v>0</v>
       </c>
       <c r="F125" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
@@ -6067,7 +6058,7 @@
         <v>219</v>
       </c>
       <c r="B126" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D126" t="b">
         <v>0</v>
@@ -6078,7 +6069,7 @@
         <v>181</v>
       </c>
       <c r="B127" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D127" t="b">
         <v>0</v>
@@ -6089,7 +6080,7 @@
         <v>185</v>
       </c>
       <c r="B128" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D128" t="b">
         <v>0</v>
@@ -6100,7 +6091,7 @@
         <v>177</v>
       </c>
       <c r="B129" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D129" t="b">
         <v>0</v>
@@ -6111,13 +6102,13 @@
         <v>209</v>
       </c>
       <c r="B130" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D130" t="b">
         <v>0</v>
       </c>
       <c r="H130" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
@@ -6125,7 +6116,7 @@
         <v>178</v>
       </c>
       <c r="B131" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D131" t="b">
         <v>0</v>
@@ -6136,7 +6127,7 @@
         <v>179</v>
       </c>
       <c r="B132" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D132" t="b">
         <v>0</v>
@@ -6147,7 +6138,7 @@
         <v>221</v>
       </c>
       <c r="B133" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D133" t="b">
         <v>0</v>
@@ -6158,7 +6149,7 @@
         <v>206</v>
       </c>
       <c r="B134" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D134" t="b">
         <v>0</v>
@@ -6169,7 +6160,7 @@
         <v>229</v>
       </c>
       <c r="B135" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D135" t="b">
         <v>0</v>
@@ -6180,7 +6171,7 @@
         <v>187</v>
       </c>
       <c r="B136" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D136" t="b">
         <v>0</v>
@@ -6191,7 +6182,7 @@
         <v>205</v>
       </c>
       <c r="B137" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D137" t="b">
         <v>0</v>
@@ -6202,7 +6193,7 @@
         <v>193</v>
       </c>
       <c r="B138" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D138" t="b">
         <v>0</v>
@@ -6213,7 +6204,7 @@
         <v>190</v>
       </c>
       <c r="B139" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D139" t="b">
         <v>0</v>
@@ -6224,7 +6215,7 @@
         <v>210</v>
       </c>
       <c r="B140" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D140" t="b">
         <v>0</v>
@@ -6235,7 +6226,7 @@
         <v>230</v>
       </c>
       <c r="B141" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D141" t="b">
         <v>0</v>
@@ -6246,16 +6237,16 @@
         <v>106</v>
       </c>
       <c r="B142" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C142" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F142" t="s">
         <v>245</v>
       </c>
       <c r="G142" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
@@ -6263,10 +6254,10 @@
         <v>98</v>
       </c>
       <c r="B143" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C143" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F143" t="s">
         <v>246</v>
@@ -6280,10 +6271,10 @@
         <v>10</v>
       </c>
       <c r="B144" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C144" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F144" t="s">
         <v>245</v>
@@ -6297,10 +6288,10 @@
         <v>159</v>
       </c>
       <c r="B145" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C145" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F145" t="s">
         <v>257</v>
@@ -6314,10 +6305,10 @@
         <v>49</v>
       </c>
       <c r="B146" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C146" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F146" t="s">
         <v>240</v>
@@ -6331,10 +6322,10 @@
         <v>137</v>
       </c>
       <c r="B147" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C147" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F147" t="s">
         <v>242</v>
@@ -6348,10 +6339,10 @@
         <v>90</v>
       </c>
       <c r="B148" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C148" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F148" t="s">
         <v>246</v>
@@ -6365,10 +6356,10 @@
         <v>87</v>
       </c>
       <c r="B149" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C149" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F149" t="s">
         <v>246</v>
@@ -6382,10 +6373,10 @@
         <v>173</v>
       </c>
       <c r="B150" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C150" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F150" t="s">
         <v>240</v>
@@ -6399,10 +6390,10 @@
         <v>134</v>
       </c>
       <c r="B151" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C151" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F151" t="s">
         <v>242</v>
@@ -6416,10 +6407,10 @@
         <v>144</v>
       </c>
       <c r="B152" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C152" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F152" t="s">
         <v>245</v>
@@ -6433,10 +6424,10 @@
         <v>166</v>
       </c>
       <c r="B153" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C153" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F153" t="s">
         <v>245</v>
@@ -6450,10 +6441,10 @@
         <v>50</v>
       </c>
       <c r="B154" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C154" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F154" t="s">
         <v>240</v>
@@ -6467,10 +6458,10 @@
         <v>168</v>
       </c>
       <c r="B155" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C155" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F155" t="s">
         <v>252</v>
@@ -6484,10 +6475,10 @@
         <v>94</v>
       </c>
       <c r="B156" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C156" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F156" t="s">
         <v>240</v>
@@ -6501,10 +6492,10 @@
         <v>176</v>
       </c>
       <c r="B157" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C157" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F157" t="s">
         <v>240</v>
@@ -6518,10 +6509,10 @@
         <v>51</v>
       </c>
       <c r="B158" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C158" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F158" t="s">
         <v>240</v>
@@ -6535,10 +6526,10 @@
         <v>155</v>
       </c>
       <c r="B159" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C159" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F159" t="s">
         <v>240</v>
@@ -6552,10 +6543,10 @@
         <v>142</v>
       </c>
       <c r="B160" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C160" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F160" t="s">
         <v>242</v>
@@ -6569,10 +6560,10 @@
         <v>138</v>
       </c>
       <c r="B161" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C161" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F161" t="s">
         <v>248</v>
@@ -6586,10 +6577,10 @@
         <v>149</v>
       </c>
       <c r="B162" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C162" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F162" t="s">
         <v>248</v>
@@ -6603,10 +6594,10 @@
         <v>174</v>
       </c>
       <c r="B163" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C163" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F163" t="s">
         <v>252</v>
@@ -6620,10 +6611,10 @@
         <v>82</v>
       </c>
       <c r="B164" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C164" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F164" t="s">
         <v>240</v>
@@ -6637,10 +6628,10 @@
         <v>71</v>
       </c>
       <c r="B165" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C165" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F165" t="s">
         <v>240</v>
@@ -6654,10 +6645,10 @@
         <v>74</v>
       </c>
       <c r="B166" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C166" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F166" t="s">
         <v>240</v>
@@ -6671,10 +6662,10 @@
         <v>156</v>
       </c>
       <c r="B167" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C167" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F167" t="s">
         <v>242</v>
@@ -6688,13 +6679,13 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C168" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F168" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G168" t="s">
         <v>239</v>
@@ -6705,10 +6696,10 @@
         <v>23</v>
       </c>
       <c r="B169" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C169" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F169" t="s">
         <v>240</v>
@@ -6722,10 +6713,10 @@
         <v>164</v>
       </c>
       <c r="B170" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C170" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F170" t="s">
         <v>248</v>
@@ -6739,10 +6730,10 @@
         <v>115</v>
       </c>
       <c r="B171" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C171" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F171" t="s">
         <v>250</v>
@@ -6756,10 +6747,10 @@
         <v>57</v>
       </c>
       <c r="B172" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C172" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F172" t="s">
         <v>240</v>
@@ -6773,10 +6764,10 @@
         <v>95</v>
       </c>
       <c r="B173" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C173" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F173" t="s">
         <v>240</v>
@@ -6790,10 +6781,10 @@
         <v>161</v>
       </c>
       <c r="B174" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C174" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F174" t="s">
         <v>248</v>
@@ -6807,10 +6798,10 @@
         <v>109</v>
       </c>
       <c r="B175" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C175" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F175" t="s">
         <v>246</v>
@@ -6824,10 +6815,10 @@
         <v>92</v>
       </c>
       <c r="B176" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C176" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F176" t="s">
         <v>240</v>
@@ -6841,10 +6832,10 @@
         <v>64</v>
       </c>
       <c r="B177" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C177" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F177" t="s">
         <v>240</v>
@@ -6858,10 +6849,10 @@
         <v>99</v>
       </c>
       <c r="B178" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C178" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F178" t="s">
         <v>257</v>
@@ -6875,10 +6866,10 @@
         <v>163</v>
       </c>
       <c r="B179" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C179" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F179" t="s">
         <v>252</v>
@@ -6892,10 +6883,10 @@
         <v>66</v>
       </c>
       <c r="B180" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C180" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F180" t="s">
         <v>245</v>
@@ -6909,10 +6900,10 @@
         <v>158</v>
       </c>
       <c r="B181" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C181" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F181" t="s">
         <v>257</v>
@@ -6926,10 +6917,10 @@
         <v>114</v>
       </c>
       <c r="B182" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C182" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F182" t="s">
         <v>242</v>
@@ -6943,10 +6934,10 @@
         <v>18</v>
       </c>
       <c r="B183" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C183" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F183" t="s">
         <v>240</v>
@@ -6960,10 +6951,10 @@
         <v>110</v>
       </c>
       <c r="B184" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C184" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F184" t="s">
         <v>242</v>
@@ -6977,10 +6968,10 @@
         <v>224</v>
       </c>
       <c r="B185" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C185" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D185" t="b">
         <v>0</v>
@@ -6997,10 +6988,10 @@
         <v>72</v>
       </c>
       <c r="B186" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C186" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F186" t="s">
         <v>240</v>
@@ -7014,10 +7005,10 @@
         <v>1</v>
       </c>
       <c r="B187" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C187" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F187" t="s">
         <v>240</v>
@@ -7031,10 +7022,10 @@
         <v>140</v>
       </c>
       <c r="B188" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C188" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F188" t="s">
         <v>240</v>
@@ -7048,10 +7039,10 @@
         <v>154</v>
       </c>
       <c r="B189" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C189" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F189" t="s">
         <v>240</v>
@@ -7065,10 +7056,10 @@
         <v>175</v>
       </c>
       <c r="B190" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C190" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F190" t="s">
         <v>242</v>
@@ -7082,10 +7073,10 @@
         <v>143</v>
       </c>
       <c r="B191" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C191" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F191" t="s">
         <v>240</v>
@@ -7099,10 +7090,10 @@
         <v>83</v>
       </c>
       <c r="B192" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C192" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F192" t="s">
         <v>253</v>
@@ -7116,10 +7107,10 @@
         <v>86</v>
       </c>
       <c r="B193" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C193" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F193" t="s">
         <v>240</v>
@@ -7133,10 +7124,10 @@
         <v>145</v>
       </c>
       <c r="B194" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C194" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F194" t="s">
         <v>240</v>
@@ -7150,10 +7141,10 @@
         <v>151</v>
       </c>
       <c r="B195" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C195" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F195" t="s">
         <v>240</v>
@@ -7167,10 +7158,10 @@
         <v>48</v>
       </c>
       <c r="B196" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C196" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F196" t="s">
         <v>248</v>
@@ -7184,10 +7175,10 @@
         <v>111</v>
       </c>
       <c r="B197" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C197" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F197" t="s">
         <v>240</v>
@@ -7201,10 +7192,10 @@
         <v>93</v>
       </c>
       <c r="B198" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C198" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F198" t="s">
         <v>240</v>
@@ -7218,10 +7209,10 @@
         <v>150</v>
       </c>
       <c r="B199" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C199" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F199" t="s">
         <v>248</v>
@@ -7235,13 +7226,13 @@
         <v>171</v>
       </c>
       <c r="B200" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C200" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F200" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G200" t="s">
         <v>241</v>
@@ -7252,10 +7243,10 @@
         <v>100</v>
       </c>
       <c r="B201" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C201" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F201" t="s">
         <v>240</v>
@@ -7269,10 +7260,10 @@
         <v>165</v>
       </c>
       <c r="B202" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C202" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F202" t="s">
         <v>242</v>
@@ -7286,10 +7277,10 @@
         <v>113</v>
       </c>
       <c r="B203" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C203" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F203" t="s">
         <v>240</v>
@@ -7303,10 +7294,10 @@
         <v>75</v>
       </c>
       <c r="B204" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C204" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F204" t="s">
         <v>242</v>
@@ -7320,10 +7311,10 @@
         <v>31</v>
       </c>
       <c r="B205" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C205" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F205" t="s">
         <v>240</v>
@@ -7337,10 +7328,10 @@
         <v>204</v>
       </c>
       <c r="B206" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C206" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D206" t="b">
         <v>0</v>
@@ -7351,16 +7342,16 @@
         <v>213</v>
       </c>
       <c r="B207" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C207" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D207" t="b">
         <v>0</v>
       </c>
       <c r="H207" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
@@ -7368,10 +7359,10 @@
         <v>184</v>
       </c>
       <c r="B208" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C208" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D208" t="b">
         <v>0</v>
@@ -7382,10 +7373,10 @@
         <v>215</v>
       </c>
       <c r="B209" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C209" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D209" t="b">
         <v>0</v>
@@ -7396,10 +7387,10 @@
         <v>71</v>
       </c>
       <c r="B210" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C210" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D210" t="b">
         <v>0</v>
@@ -7410,10 +7401,10 @@
         <v>202</v>
       </c>
       <c r="B211" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C211" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D211" t="b">
         <v>0</v>
@@ -7424,10 +7415,10 @@
         <v>220</v>
       </c>
       <c r="B212" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C212" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D212" t="b">
         <v>0</v>
@@ -7438,10 +7429,10 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C213" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D213" t="b">
         <v>0</v>
@@ -7452,10 +7443,10 @@
         <v>214</v>
       </c>
       <c r="B214" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C214" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D214" t="b">
         <v>0</v>
@@ -7466,10 +7457,10 @@
         <v>198</v>
       </c>
       <c r="B215" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C215" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D215" t="b">
         <v>0</v>
@@ -7480,10 +7471,10 @@
         <v>228</v>
       </c>
       <c r="B216" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C216" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D216" t="b">
         <v>0</v>
@@ -7494,10 +7485,10 @@
         <v>180</v>
       </c>
       <c r="B217" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C217" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D217" t="b">
         <v>0</v>
@@ -7508,10 +7499,10 @@
         <v>189</v>
       </c>
       <c r="B218" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C218" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D218" t="b">
         <v>0</v>
@@ -7522,10 +7513,10 @@
         <v>188</v>
       </c>
       <c r="B219" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C219" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D219" t="b">
         <v>0</v>
@@ -7536,10 +7527,10 @@
         <v>199</v>
       </c>
       <c r="B220" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C220" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D220" t="b">
         <v>0</v>
@@ -7550,10 +7541,10 @@
         <v>195</v>
       </c>
       <c r="B221" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C221" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D221" t="b">
         <v>0</v>
@@ -7564,10 +7555,10 @@
         <v>201</v>
       </c>
       <c r="B222" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C222" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D222" t="b">
         <v>0</v>
@@ -7578,10 +7569,10 @@
         <v>69</v>
       </c>
       <c r="B223" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C223" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F223" t="s">
         <v>240</v>
@@ -7726,7 +7717,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H239" xr:uid="{4629592B-0E0F-485D-B1E6-ECE7C0C63CAD}"/>
+  <autoFilter ref="A1:H235" xr:uid="{4629592B-0E0F-485D-B1E6-ECE7C0C63CAD}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H238">
     <sortCondition ref="B2:B238"/>
     <sortCondition ref="C2:C238"/>
@@ -7741,7 +7732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02E585C-7598-487E-8D13-D59FA603C0B2}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -7762,7 +7753,7 @@
         <v>233</v>
       </c>
       <c r="B1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -7770,26 +7761,26 @@
         <v>234</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B5" t="s">
         <v>251</v>
       </c>
       <c r="C5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D5" t="s">
         <v>243</v>
@@ -7807,15 +7798,15 @@
         <v>249</v>
       </c>
       <c r="I5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -7833,7 +7824,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
@@ -7861,7 +7852,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
@@ -7887,7 +7878,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -7911,7 +7902,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -7925,7 +7916,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -7979,7 +7970,7 @@
         <v>251</v>
       </c>
       <c r="C19" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D19" t="s">
         <v>243</v>
@@ -7988,13 +7979,13 @@
         <v>247</v>
       </c>
       <c r="F19" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G19" t="s">
         <v>239</v>
       </c>
       <c r="H19" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="I19" t="s">
         <v>241</v>
@@ -8080,18 +8071,18 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G28" t="s">
         <v>239</v>
       </c>
       <c r="H28" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F29">
         <v>16</v>
@@ -8105,7 +8096,7 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F30">
         <v>11</v>
@@ -8119,7 +8110,7 @@
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E31" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F31">
         <v>3</v>
@@ -8133,7 +8124,7 @@
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E32" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F32">
         <v>1</v>

</xml_diff>